<commit_message>
[#79026726] traffic styling and legends
</commit_message>
<xml_diff>
--- a/public/assets/img/map_legends/percentiles.xlsx
+++ b/public/assets/img/map_legends/percentiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="4100" windowWidth="27440" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="12400" yWindow="4000" windowWidth="27440" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Percentile</t>
   </si>
@@ -40,13 +40,28 @@
   </si>
   <si>
     <t>40 to 60 (Middle 20%)</t>
+  </si>
+  <si>
+    <t>This year</t>
+  </si>
+  <si>
+    <t>Last year</t>
+  </si>
+  <si>
+    <t>Two to three years ago</t>
+  </si>
+  <si>
+    <t>Four to five years ago</t>
+  </si>
+  <si>
+    <t>More than five years ago</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,6 +84,29 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,10 +165,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -141,8 +195,25 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -590,7 +661,100 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="20">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="20">
+      <c r="A16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="20">
+      <c r="A17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="20">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="20">
+      <c r="A19" s="7"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="20">
+      <c r="A20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
     </row>
   </sheetData>
   <customSheetViews>

</xml_diff>